<commit_message>
backup file for csv
</commit_message>
<xml_diff>
--- a/data/expenses.xlsx
+++ b/data/expenses.xlsx
@@ -1,47 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skm/Documents/MHCI/Summer 2021/HCI 584/Project/grocery-spending_skmorris/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEF2309-723B-5D4B-BF8F-E64044D26F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43692B44-65CB-F041-82BD-A393B677342A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="500" windowWidth="27240" windowHeight="20640" xr2:uid="{D2050EBE-C9BB-6F4B-A1EA-6BA6AB59931E}"/>
+    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="expenses" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="40">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Purchase Date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="41">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Sparkling Water</t>
+  </si>
+  <si>
+    <t>Beverages</t>
   </si>
   <si>
     <t>2% Milk</t>
   </si>
   <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Hot Dogs</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Strawberries</t>
+  </si>
+  <si>
+    <t>Produce</t>
+  </si>
+  <si>
     <t>Cheetos</t>
   </si>
   <si>
+    <t>Snacks</t>
+  </si>
+  <si>
     <t>Cool Ranch Doritos</t>
   </si>
   <si>
@@ -54,7 +79,7 @@
     <t>Gummy Bears</t>
   </si>
   <si>
-    <t>Hot Dogs</t>
+    <t>Candy</t>
   </si>
   <si>
     <t>Oreo Cookies</t>
@@ -63,95 +88,71 @@
     <t>Reese's Cups</t>
   </si>
   <si>
-    <t>Sparkling Water</t>
-  </si>
-  <si>
-    <t>Strawberries</t>
-  </si>
-  <si>
     <t>Twizzlers</t>
   </si>
   <si>
+    <t>Energy Drinks</t>
+  </si>
+  <si>
+    <t>Chicken Breast</t>
+  </si>
+  <si>
+    <t>Broccoli</t>
+  </si>
+  <si>
+    <t>Animal Crackers</t>
+  </si>
+  <si>
+    <t>Cheez-It Crackers</t>
+  </si>
+  <si>
+    <t>Lays Potato Chips</t>
+  </si>
+  <si>
+    <t>Diet Coke</t>
+  </si>
+  <si>
+    <t>Sharp Cheddar Cheese</t>
+  </si>
+  <si>
+    <t>Carrots</t>
+  </si>
+  <si>
+    <t>Romaine Lettuce</t>
+  </si>
+  <si>
     <t>Goldfish</t>
   </si>
   <si>
-    <t>Lays Potato Chips</t>
-  </si>
-  <si>
-    <t>Animal Crackers</t>
-  </si>
-  <si>
-    <t>Broccoli</t>
-  </si>
-  <si>
-    <t>Cheez-It Crackers</t>
-  </si>
-  <si>
-    <t>Chicken Breast</t>
-  </si>
-  <si>
-    <t>Energy Drinks</t>
+    <t>Hazelnut Coffee Creamer</t>
+  </si>
+  <si>
+    <t>Pork Chops</t>
   </si>
   <si>
     <t>Chex Mix</t>
   </si>
   <si>
-    <t>Hazelnut Coffee Creamer</t>
-  </si>
-  <si>
-    <t>Pork Chops</t>
+    <t>Sour Cream</t>
+  </si>
+  <si>
+    <t>Ground Beef</t>
   </si>
   <si>
     <t>Asparagus</t>
   </si>
   <si>
-    <t>Ground Beef</t>
-  </si>
-  <si>
-    <t>Sour Cream</t>
-  </si>
-  <si>
-    <t>Carrots</t>
-  </si>
-  <si>
-    <t>Diet Coke</t>
-  </si>
-  <si>
-    <t>Romaine Lettuce</t>
-  </si>
-  <si>
-    <t>Sharp Cheddar Cheese</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Dairy</t>
-  </si>
-  <si>
-    <t>Snacks</t>
-  </si>
-  <si>
-    <t>Produce</t>
-  </si>
-  <si>
-    <t>Beverages</t>
-  </si>
-  <si>
-    <t>Meat</t>
-  </si>
-  <si>
-    <t>Candy</t>
+    <t>Brownies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,21 +161,315 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -182,26 +477,207 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -212,23 +688,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0157B22-996F-CA44-A2F6-F50717EB2691}" name="Table13" displayName="Table13" ref="A1:E62" totalsRowShown="0">
-  <autoFilter ref="A1:E62" xr:uid="{D1873461-B999-D24B-AE72-63EF2CC3E0E9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E62">
-    <sortCondition ref="E1:E62"/>
-  </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2E28355B-C5D4-7743-A89E-424AD687818A}" name="Name"/>
-    <tableColumn id="8" xr3:uid="{D0BB7303-565E-0B4A-99FF-EF825ACC6856}" name="Category"/>
-    <tableColumn id="9" xr3:uid="{6383D132-3D98-BB41-9C60-D2165371CB12}" name="Price" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{47D3AE7F-1E5A-A848-B737-448CC3028E69}" name="Quantity"/>
-    <tableColumn id="5" xr3:uid="{AD7E8924-73FD-7A4D-B815-9F81396B8CDA}" name="Purchase Date" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,21 +986,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F974CEF9-8B40-AA43-8CA6-DF119D30DF12}">
-  <dimension ref="A1:E62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:B62"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -549,26 +1003,26 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="2">
+        <v>6</v>
+      </c>
+      <c r="C2">
         <v>5.79</v>
       </c>
       <c r="D2">
@@ -580,12 +1034,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>2.59</v>
       </c>
       <c r="D3">
@@ -600,9 +1054,9 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4">
         <v>3.99</v>
       </c>
       <c r="D4">
@@ -614,12 +1068,12 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="2">
+        <v>12</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
@@ -631,12 +1085,12 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="2">
+        <v>14</v>
+      </c>
+      <c r="C6">
         <v>3.49</v>
       </c>
       <c r="D6">
@@ -648,12 +1102,12 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2">
+        <v>14</v>
+      </c>
+      <c r="C7">
         <v>4.29</v>
       </c>
       <c r="D7">
@@ -665,12 +1119,12 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2">
+        <v>14</v>
+      </c>
+      <c r="C8">
         <v>3.49</v>
       </c>
       <c r="D8">
@@ -682,12 +1136,12 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="2">
+        <v>14</v>
+      </c>
+      <c r="C9">
         <v>3.79</v>
       </c>
       <c r="D9">
@@ -699,12 +1153,12 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="2">
+        <v>19</v>
+      </c>
+      <c r="C10">
         <v>1.99</v>
       </c>
       <c r="D10">
@@ -716,12 +1170,12 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2">
+        <v>14</v>
+      </c>
+      <c r="C11">
         <v>3.19</v>
       </c>
       <c r="D11">
@@ -733,12 +1187,12 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2">
+        <v>19</v>
+      </c>
+      <c r="C12">
         <v>1.19</v>
       </c>
       <c r="D12">
@@ -750,12 +1204,12 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2">
+        <v>19</v>
+      </c>
+      <c r="C13">
         <v>1.99</v>
       </c>
       <c r="D13">
@@ -767,12 +1221,12 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14">
         <v>8.49</v>
       </c>
       <c r="D14">
@@ -784,12 +1238,12 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="2">
+        <v>10</v>
+      </c>
+      <c r="C15">
         <v>6.29</v>
       </c>
       <c r="D15">
@@ -801,12 +1255,12 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="2">
+        <v>12</v>
+      </c>
+      <c r="C16">
         <v>2.5</v>
       </c>
       <c r="D16">
@@ -818,12 +1272,12 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2">
+        <v>14</v>
+      </c>
+      <c r="C17">
         <v>3.99</v>
       </c>
       <c r="D17">
@@ -835,12 +1289,12 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="2">
+        <v>14</v>
+      </c>
+      <c r="C18">
         <v>2.5</v>
       </c>
       <c r="D18">
@@ -852,12 +1306,12 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="2">
+        <v>14</v>
+      </c>
+      <c r="C19">
         <v>4.29</v>
       </c>
       <c r="D19">
@@ -869,12 +1323,12 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20">
         <v>1.99</v>
       </c>
       <c r="D20">
@@ -886,12 +1340,12 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="2">
+        <v>14</v>
+      </c>
+      <c r="C21">
         <v>3.99</v>
       </c>
       <c r="D21">
@@ -903,12 +1357,12 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="2">
+        <v>14</v>
+      </c>
+      <c r="C22">
         <v>3.99</v>
       </c>
       <c r="D22">
@@ -920,12 +1374,12 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="2">
+        <v>19</v>
+      </c>
+      <c r="C23">
         <v>1.19</v>
       </c>
       <c r="D23">
@@ -940,9 +1394,9 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="2">
+        <v>6</v>
+      </c>
+      <c r="C24">
         <v>6.49</v>
       </c>
       <c r="D24">
@@ -954,12 +1408,12 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="2">
+        <v>6</v>
+      </c>
+      <c r="C25">
         <v>5.79</v>
       </c>
       <c r="D25">
@@ -971,12 +1425,12 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="2">
+        <v>8</v>
+      </c>
+      <c r="C26">
         <v>3.49</v>
       </c>
       <c r="D26">
@@ -988,12 +1442,12 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="2">
+        <v>12</v>
+      </c>
+      <c r="C27">
         <v>2.99</v>
       </c>
       <c r="D27">
@@ -1005,12 +1459,12 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="2">
+        <v>12</v>
+      </c>
+      <c r="C28">
         <v>2.4900000000000002</v>
       </c>
       <c r="D28">
@@ -1022,12 +1476,12 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="2">
+        <v>14</v>
+      </c>
+      <c r="C29">
         <v>3.99</v>
       </c>
       <c r="D29">
@@ -1039,12 +1493,12 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="2">
+        <v>14</v>
+      </c>
+      <c r="C30">
         <v>2.99</v>
       </c>
       <c r="D30">
@@ -1056,12 +1510,12 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="2">
+        <v>19</v>
+      </c>
+      <c r="C31">
         <v>1.99</v>
       </c>
       <c r="D31">
@@ -1073,12 +1527,12 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="2">
+        <v>14</v>
+      </c>
+      <c r="C32">
         <v>3.19</v>
       </c>
       <c r="D32">
@@ -1090,12 +1544,12 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="2">
+        <v>19</v>
+      </c>
+      <c r="C33">
         <v>1.19</v>
       </c>
       <c r="D33">
@@ -1107,12 +1561,12 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="2">
+        <v>6</v>
+      </c>
+      <c r="C34">
         <v>5.79</v>
       </c>
       <c r="D34">
@@ -1124,12 +1578,12 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="2">
+        <v>8</v>
+      </c>
+      <c r="C35">
         <v>2.59</v>
       </c>
       <c r="D35">
@@ -1141,12 +1595,12 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="2">
+        <v>14</v>
+      </c>
+      <c r="C36">
         <v>4.29</v>
       </c>
       <c r="D36">
@@ -1158,12 +1612,12 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="2">
+        <v>14</v>
+      </c>
+      <c r="C37">
         <v>2.99</v>
       </c>
       <c r="D37">
@@ -1175,12 +1629,12 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="2">
+        <v>19</v>
+      </c>
+      <c r="C38">
         <v>1.99</v>
       </c>
       <c r="D38">
@@ -1192,12 +1646,12 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="2">
+        <v>14</v>
+      </c>
+      <c r="C39">
         <v>3.99</v>
       </c>
       <c r="D39">
@@ -1209,12 +1663,12 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="2">
+        <v>14</v>
+      </c>
+      <c r="C40">
         <v>3.19</v>
       </c>
       <c r="D40">
@@ -1226,12 +1680,12 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="2">
+        <v>19</v>
+      </c>
+      <c r="C41">
         <v>1.19</v>
       </c>
       <c r="D41">
@@ -1243,12 +1697,12 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="2">
+        <v>19</v>
+      </c>
+      <c r="C42">
         <v>1.99</v>
       </c>
       <c r="D42">
@@ -1260,12 +1714,12 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="2">
+        <v>6</v>
+      </c>
+      <c r="C43">
         <v>8.49</v>
       </c>
       <c r="D43">
@@ -1277,12 +1731,12 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="2">
+        <v>8</v>
+      </c>
+      <c r="C44">
         <v>3.79</v>
       </c>
       <c r="D44">
@@ -1294,12 +1748,12 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="2">
+        <v>10</v>
+      </c>
+      <c r="C45">
         <v>6.99</v>
       </c>
       <c r="D45">
@@ -1311,12 +1765,12 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="2">
+        <v>12</v>
+      </c>
+      <c r="C46">
         <v>2.5</v>
       </c>
       <c r="D46">
@@ -1328,12 +1782,12 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="2">
+        <v>14</v>
+      </c>
+      <c r="C47">
         <v>2.5</v>
       </c>
       <c r="D47">
@@ -1345,12 +1799,12 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="2">
+        <v>14</v>
+      </c>
+      <c r="C48">
         <v>1.39</v>
       </c>
       <c r="D48">
@@ -1362,12 +1816,12 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="2">
+        <v>14</v>
+      </c>
+      <c r="C49">
         <v>3.79</v>
       </c>
       <c r="D49">
@@ -1379,12 +1833,12 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="2">
+        <v>19</v>
+      </c>
+      <c r="C50">
         <v>1.99</v>
       </c>
       <c r="D50">
@@ -1396,12 +1850,12 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="2">
+        <v>14</v>
+      </c>
+      <c r="C51">
         <v>3.99</v>
       </c>
       <c r="D51">
@@ -1413,12 +1867,12 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
-      </c>
-      <c r="C52" s="2">
+        <v>19</v>
+      </c>
+      <c r="C52">
         <v>1.19</v>
       </c>
       <c r="D52">
@@ -1430,12 +1884,12 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C53" s="2">
+        <v>6</v>
+      </c>
+      <c r="C53">
         <v>8.49</v>
       </c>
       <c r="D53">
@@ -1447,12 +1901,12 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
-      </c>
-      <c r="C54" s="2">
+        <v>6</v>
+      </c>
+      <c r="C54">
         <v>5.79</v>
       </c>
       <c r="D54">
@@ -1464,12 +1918,12 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="2">
+        <v>8</v>
+      </c>
+      <c r="C55">
         <v>1.99</v>
       </c>
       <c r="D55">
@@ -1481,12 +1935,12 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" s="2">
+        <v>10</v>
+      </c>
+      <c r="C56">
         <v>6.99</v>
       </c>
       <c r="D56">
@@ -1498,12 +1952,12 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="2">
+        <v>12</v>
+      </c>
+      <c r="C57">
         <v>2.99</v>
       </c>
       <c r="D57">
@@ -1515,12 +1969,12 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
-      </c>
-      <c r="C58" s="2">
+        <v>14</v>
+      </c>
+      <c r="C58">
         <v>3.49</v>
       </c>
       <c r="D58">
@@ -1532,12 +1986,12 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="2">
+        <v>14</v>
+      </c>
+      <c r="C59">
         <v>1.39</v>
       </c>
       <c r="D59">
@@ -1549,12 +2003,12 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
-      </c>
-      <c r="C60" s="2">
+        <v>14</v>
+      </c>
+      <c r="C60">
         <v>2.99</v>
       </c>
       <c r="D60">
@@ -1566,12 +2020,12 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="2">
+        <v>19</v>
+      </c>
+      <c r="C61">
         <v>1.99</v>
       </c>
       <c r="D61">
@@ -1583,12 +2037,12 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
-      </c>
-      <c r="C62" s="2">
+        <v>19</v>
+      </c>
+      <c r="C62">
         <v>1.19</v>
       </c>
       <c r="D62">
@@ -1598,11 +2052,41 @@
         <v>44375</v>
       </c>
     </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63">
+        <v>4.49</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1">
+        <v>44368</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>1.99</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1">
+        <v>44368</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>